<commit_message>
ITC-28 - Update Real Estate Administration template: modify `plantillaAdministracionInmuebles.xlsx`.
</commit_message>
<xml_diff>
--- a/public/templates/plantillaAdministracionInmuebles.xlsx
+++ b/public/templates/plantillaAdministracionInmuebles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrrme\Downloads\Administracion de Inmuebles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\jrrmelecio\projects\itc-pld\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B2E42C-A838-4CF7-ABD0-7E3F989DEF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B647512-030C-4C92-86B3-D861C5203416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="6" r:id="rId1"/>
@@ -2810,7 +2810,7 @@
     <t>Denominacion</t>
   </si>
   <si>
-    <t>Datos Unicos Por Persona Obejeto del Aviso</t>
+    <t>Datos Unicos Por Persona Objeto del Aviso</t>
   </si>
 </sst>
 </file>
@@ -3058,13 +3058,11 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3073,7 +3071,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3353,7 +3353,7 @@
   <dimension ref="A1:BT103"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="BC1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BF7" sqref="BF7"/>
+      <selection activeCell="BF3" sqref="BF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -3432,79 +3432,79 @@
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>922</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
+      <c r="AM1" s="16"/>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="16"/>
       <c r="AQ1" s="18"/>
-      <c r="AR1" s="14" t="s">
+      <c r="AR1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-      <c r="BB1" s="15"/>
-      <c r="BC1" s="15"/>
-      <c r="BD1" s="15"/>
+      <c r="AS1" s="16"/>
+      <c r="AT1" s="16"/>
+      <c r="AU1" s="16"/>
+      <c r="AV1" s="16"/>
+      <c r="AW1" s="16"/>
+      <c r="AX1" s="16"/>
+      <c r="AY1" s="16"/>
+      <c r="AZ1" s="16"/>
+      <c r="BA1" s="16"/>
+      <c r="BB1" s="16"/>
+      <c r="BC1" s="16"/>
+      <c r="BD1" s="16"/>
       <c r="BE1" s="18"/>
       <c r="BF1" s="13"/>
       <c r="BG1" s="13"/>
-      <c r="BH1" s="14"/>
-      <c r="BI1" s="15"/>
-      <c r="BJ1" s="15"/>
-      <c r="BK1" s="15"/>
-      <c r="BL1" s="15"/>
-      <c r="BM1" s="15"/>
-      <c r="BN1" s="15"/>
-      <c r="BO1" s="15"/>
-      <c r="BP1" s="15"/>
-      <c r="BQ1" s="15"/>
-      <c r="BR1" s="15"/>
-      <c r="BS1" s="15"/>
-      <c r="BT1" s="15"/>
+      <c r="BH1" s="15"/>
+      <c r="BI1" s="16"/>
+      <c r="BJ1" s="16"/>
+      <c r="BK1" s="16"/>
+      <c r="BL1" s="16"/>
+      <c r="BM1" s="16"/>
+      <c r="BN1" s="16"/>
+      <c r="BO1" s="16"/>
+      <c r="BP1" s="16"/>
+      <c r="BQ1" s="16"/>
+      <c r="BR1" s="16"/>
+      <c r="BS1" s="16"/>
+      <c r="BT1" s="16"/>
     </row>
     <row r="2" spans="1:72" ht="15.75" thickBot="1">
       <c r="A2" s="17" t="s">
@@ -3512,99 +3512,99 @@
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
       <c r="K2" s="18"/>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="14" t="s">
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="14" t="s">
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="14" t="s">
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="14" t="s">
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="15" t="s">
         <v>924</v>
       </c>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="16"/>
-      <c r="AO2" s="14" t="s">
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="16"/>
+      <c r="AK2" s="16"/>
+      <c r="AL2" s="16"/>
+      <c r="AM2" s="16"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="14" t="s">
+      <c r="AP2" s="16"/>
+      <c r="AQ2" s="16"/>
+      <c r="AR2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AS2" s="15"/>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15"/>
-      <c r="AV2" s="15"/>
-      <c r="AW2" s="15"/>
-      <c r="AX2" s="16"/>
-      <c r="AY2" s="14" t="s">
+      <c r="AS2" s="16"/>
+      <c r="AT2" s="16"/>
+      <c r="AU2" s="16"/>
+      <c r="AV2" s="16"/>
+      <c r="AW2" s="16"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="AZ2" s="15"/>
-      <c r="BA2" s="15"/>
-      <c r="BB2" s="15"/>
-      <c r="BC2" s="14" t="s">
+      <c r="AZ2" s="16"/>
+      <c r="BA2" s="16"/>
+      <c r="BB2" s="16"/>
+      <c r="BC2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="BD2" s="15"/>
-      <c r="BE2" s="15"/>
-      <c r="BF2" s="14" t="s">
+      <c r="BD2" s="16"/>
+      <c r="BE2" s="16"/>
+      <c r="BF2" s="15" t="s">
         <v>927</v>
       </c>
       <c r="BG2" s="18"/>
-      <c r="BH2" s="14" t="s">
+      <c r="BH2" s="15" t="s">
         <v>920</v>
       </c>
-      <c r="BI2" s="15"/>
-      <c r="BJ2" s="15"/>
-      <c r="BK2" s="15"/>
-      <c r="BL2" s="15"/>
-      <c r="BM2" s="15"/>
-      <c r="BN2" s="15"/>
-      <c r="BO2" s="15"/>
-      <c r="BP2" s="15"/>
-      <c r="BQ2" s="15"/>
-      <c r="BR2" s="15"/>
-      <c r="BS2" s="15"/>
-      <c r="BT2" s="15"/>
+      <c r="BI2" s="16"/>
+      <c r="BJ2" s="16"/>
+      <c r="BK2" s="16"/>
+      <c r="BL2" s="16"/>
+      <c r="BM2" s="16"/>
+      <c r="BN2" s="16"/>
+      <c r="BO2" s="16"/>
+      <c r="BP2" s="16"/>
+      <c r="BQ2" s="16"/>
+      <c r="BR2" s="16"/>
+      <c r="BS2" s="16"/>
+      <c r="BT2" s="16"/>
     </row>
     <row r="3" spans="1:72" ht="15.75" thickBot="1">
       <c r="A3" s="12" t="s">
@@ -3778,10 +3778,10 @@
       <c r="BE3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="BF3" s="19" t="s">
+      <c r="BF3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="BG3" s="19" t="s">
+      <c r="BG3" s="14" t="s">
         <v>43</v>
       </c>
       <c r="BH3" s="12" t="s">
@@ -11226,6 +11226,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D1:AQ1"/>
+    <mergeCell ref="AR1:BE1"/>
     <mergeCell ref="BH1:BT1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:K2"/>
@@ -11242,8 +11244,6 @@
     <mergeCell ref="AO2:AQ2"/>
     <mergeCell ref="AR2:AX2"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:AQ1"/>
-    <mergeCell ref="AR1:BE1"/>
   </mergeCells>
   <dataValidations count="19">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L103 Q4:Q103 BC4:BC103" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -14495,12 +14495,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E59FB7EDBFDC084FA8E014A8DBC96E00" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="981b29e7ae1c4281e27c6c3ca7bd0bd5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e24eb450-30d8-45e3-917a-b05652d3d352" xmlns:ns4="ab071f45-e56c-40a0-a6d3-2085c900066c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c3148351f12fd9fea68fce5337c1368e" ns3:_="" ns4:_="">
     <xsd:import namespace="e24eb450-30d8-45e3-917a-b05652d3d352"/>
@@ -14709,6 +14703,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14719,6 +14719,12 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EDF9F43-745B-4F61-94F8-CB36D49AF3E7}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{907B828E-2CFA-4C9B-B8C0-17217CB3D2C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -14735,12 +14741,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EDF9F43-745B-4F61-94F8-CB36D49AF3E7}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F56D760F-21D1-4377-9F1B-84BA0B2ECA29}">
   <ds:schemaRefs/>

</xml_diff>

<commit_message>
ITC-28 - Update Real Estate Administration template: revise `plantillaAdministracionInmuebles.xlsx`.
</commit_message>
<xml_diff>
--- a/public/templates/plantillaAdministracionInmuebles.xlsx
+++ b/public/templates/plantillaAdministracionInmuebles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\jrrmelecio\projects\itc-pld\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B647512-030C-4C92-86B3-D861C5203416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893D8E54-37EE-4B26-94BC-C2A781166A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="929">
   <si>
     <t>RFC</t>
   </si>
@@ -2811,6 +2811,9 @@
   </si>
   <si>
     <t>Datos Unicos Por Persona Objeto del Aviso</t>
+  </si>
+  <si>
+    <t>Datos del Inmueble</t>
   </si>
 </sst>
 </file>
@@ -3065,10 +3068,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3352,8 +3355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BT103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BC1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BF3" sqref="BF3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BG1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BP13" sqref="BP13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -3427,11 +3430,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:72" ht="15.75" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="15" t="s">
         <v>922</v>
       </c>
@@ -3473,7 +3476,7 @@
       <c r="AN1" s="16"/>
       <c r="AO1" s="16"/>
       <c r="AP1" s="16"/>
-      <c r="AQ1" s="18"/>
+      <c r="AQ1" s="17"/>
       <c r="AR1" s="15" t="s">
         <v>3</v>
       </c>
@@ -3489,7 +3492,7 @@
       <c r="BB1" s="16"/>
       <c r="BC1" s="16"/>
       <c r="BD1" s="16"/>
-      <c r="BE1" s="18"/>
+      <c r="BE1" s="17"/>
       <c r="BF1" s="13"/>
       <c r="BG1" s="13"/>
       <c r="BH1" s="15"/>
@@ -3507,11 +3510,11 @@
       <c r="BT1" s="16"/>
     </row>
     <row r="2" spans="1:72" ht="15.75" thickBot="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>921</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="15" t="s">
         <v>4</v>
       </c>
@@ -3521,7 +3524,7 @@
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
-      <c r="K2" s="18"/>
+      <c r="K2" s="17"/>
       <c r="L2" s="15" t="s">
         <v>5</v>
       </c>
@@ -3589,13 +3592,15 @@
       <c r="BF2" s="15" t="s">
         <v>927</v>
       </c>
-      <c r="BG2" s="18"/>
+      <c r="BG2" s="17"/>
       <c r="BH2" s="15" t="s">
         <v>920</v>
       </c>
       <c r="BI2" s="16"/>
       <c r="BJ2" s="16"/>
-      <c r="BK2" s="16"/>
+      <c r="BK2" s="16" t="s">
+        <v>928</v>
+      </c>
       <c r="BL2" s="16"/>
       <c r="BM2" s="16"/>
       <c r="BN2" s="16"/>
@@ -11226,6 +11231,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AR2:AX2"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:AQ1"/>
     <mergeCell ref="AR1:BE1"/>
     <mergeCell ref="BH1:BT1"/>
@@ -11242,8 +11249,6 @@
     <mergeCell ref="AG2:AN2"/>
     <mergeCell ref="BF2:BG2"/>
     <mergeCell ref="AO2:AQ2"/>
-    <mergeCell ref="AR2:AX2"/>
-    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <dataValidations count="19">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L103 Q4:Q103 BC4:BC103" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -14495,6 +14500,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E59FB7EDBFDC084FA8E014A8DBC96E00" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="981b29e7ae1c4281e27c6c3ca7bd0bd5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e24eb450-30d8-45e3-917a-b05652d3d352" xmlns:ns4="ab071f45-e56c-40a0-a6d3-2085c900066c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c3148351f12fd9fea68fce5337c1368e" ns3:_="" ns4:_="">
     <xsd:import namespace="e24eb450-30d8-45e3-917a-b05652d3d352"/>
@@ -14703,12 +14714,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14719,12 +14724,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EDF9F43-745B-4F61-94F8-CB36D49AF3E7}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{907B828E-2CFA-4C9B-B8C0-17217CB3D2C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -14741,6 +14740,12 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EDF9F43-745B-4F61-94F8-CB36D49AF3E7}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F56D760F-21D1-4377-9F1B-84BA0B2ECA29}">
   <ds:schemaRefs/>

</xml_diff>